<commit_message>
TD-HBN Loss Function Fixed
</commit_message>
<xml_diff>
--- a/results/results_summary.xlsx
+++ b/results/results_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\phoenix\base\active\Class-Granular-Classifications\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8D220EA-2EB3-45D9-AD75-E99014CEE273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB049F3-E767-41C3-B805-37363078FA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E7512DF6-2F95-4E3A-81B2-878CFD547D0A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>AlexNet</t>
   </si>
@@ -50,11 +50,15 @@
     <t>Training Loss</t>
   </si>
   <si>
-    <t>Validation Accuracy</t>
+    <t xml:space="preserve">
+Note: The Super-HBN Accuracy is based on coarse classes</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Note: The Super-HBN Accuracy is based on coarse classes</t>
+    <t>TD-HBN</t>
+  </si>
+  <si>
+    <t>Validation
+Accuracy</t>
   </si>
 </sst>
 </file>
@@ -684,20 +688,20 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="60.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="62.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="6" max="6" width="60.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,18 +711,21 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="2:5" ht="259.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" ht="259.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:5" ht="289.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>4</v>
+    <row r="3" spans="2:6" ht="289.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>